<commit_message>
add villa rica campus schedules data
</commit_message>
<xml_diff>
--- a/data/horarios-de-nivelacion.xlsx
+++ b/data/horarios-de-nivelacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\fcc-pregrado-horarios-y-matriculas-xlsx-to-json\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5337226-5A74-4500-BFF0-56C42835A091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E662F1E-0A32-46DF-83C3-679E667666B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C6A9EBF-3221-4D9D-A208-CAFDA32A2193}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t>ASIGNATURAS</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>17:00-19:15</t>
+  </si>
+  <si>
+    <t>ANCAYA CORTEZ, EMILIO AGUSTÍN</t>
+  </si>
+  <si>
+    <t>16:00-18:15</t>
+  </si>
+  <si>
+    <t>OROSCO GUADALUPE, ROGER FERNANDO</t>
+  </si>
+  <si>
+    <t>15:00-17:15</t>
   </si>
 </sst>
 </file>
@@ -318,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +355,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -356,11 +374,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,13 +399,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF52B38C-8F41-4091-B166-330453BF6856}" name="Table1" displayName="Table1" ref="A1:L30" totalsRowShown="0">
-  <autoFilter ref="A1:L30" xr:uid="{FF52B38C-8F41-4091-B166-330453BF6856}">
-    <filterColumn colId="10">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L30" xr:uid="{FF52B38C-8F41-4091-B166-330453BF6856}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{B6934027-9FF7-456C-84D4-4BEA32C2C935}" name="ASIGNATURAS"/>
     <tableColumn id="2" xr3:uid="{EAD2BA29-2BD4-4B48-B0D5-AF42B0600274}" name="HORAS"/>
@@ -647,7 +660,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -703,7 +716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -733,7 +746,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -756,7 +769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -779,7 +792,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -802,7 +815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -862,7 +875,7 @@
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
@@ -890,7 +903,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -946,7 +959,7 @@
       </c>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>41</v>
       </c>
@@ -974,7 +987,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -997,24 +1010,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>3</v>
       </c>
-      <c r="C13">
-        <v>2018</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4">
+        <v>308</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1065,7 +1089,7 @@
       </c>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1088,7 +1112,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1111,7 +1135,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -1139,7 +1163,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1162,7 +1186,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1185,24 +1209,35 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>3</v>
       </c>
-      <c r="C21">
-        <v>2018</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C21" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>66</v>
       </c>
@@ -1260,7 +1295,7 @@
       </c>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -1277,7 +1312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>73</v>
       </c>
@@ -1307,7 +1342,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -1335,7 +1370,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -1358,7 +1393,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -1386,7 +1421,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>83</v>
       </c>

</xml_diff>